<commit_message>
add WDL; finished validation of deepFM & wide&deep
</commit_message>
<xml_diff>
--- a/report/model_performane.xlsx
+++ b/report/model_performane.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920"/>
+    <workbookView windowWidth="28800" windowHeight="13920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ctr_predict" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
   <si>
     <t>Hit Rate</t>
   </si>
@@ -38,6 +39,81 @@
   </si>
   <si>
     <t>something is wrong</t>
+  </si>
+  <si>
+    <t>1. deepFM &amp; wide&amp;deep got the same result -&gt; data is to small ???</t>
+  </si>
+  <si>
+    <t>logloss</t>
+  </si>
+  <si>
+    <t>model params</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model </t>
+  </si>
+  <si>
+    <t>test AUC</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>eval</t>
+  </si>
+  <si>
+    <t>optical threshold</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>layer number</t>
+  </si>
+  <si>
+    <t>neuron number</t>
+  </si>
+  <si>
+    <t>dropout</t>
+  </si>
+  <si>
+    <t>activation function</t>
+  </si>
+  <si>
+    <t>params number</t>
+  </si>
+  <si>
+    <t>dense embedding dim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wide part feature </t>
+  </si>
+  <si>
+    <t>deep part feature</t>
+  </si>
+  <si>
+    <t>deepFM</t>
+  </si>
+  <si>
+    <t>128, 128</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>26 sparse + 13 dense</t>
+  </si>
+  <si>
+    <t>wide &amp; deep</t>
+  </si>
+  <si>
+    <t>Most of the params comes from embedding: vocat_size * embdding_size * dense_feature_num</t>
   </si>
 </sst>
 </file>
@@ -45,10 +121,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -60,6 +136,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -73,11 +156,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -90,40 +173,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,25 +211,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,44 +257,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +288,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -224,13 +306,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,13 +462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,139 +474,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,17 +491,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -435,6 +508,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,6 +562,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -494,167 +585,170 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -981,18 +1075,18 @@
   <sheetPr/>
   <dimension ref="F7:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
   <sheetData>
     <row r="7" spans="8:10">
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="6:10">
       <c r="F8" t="s">
@@ -1046,4 +1140,281 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="E2:U11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
+  <cols>
+    <col min="5" max="5" width="12.9375" customWidth="1"/>
+    <col min="9" max="9" width="14.875" customWidth="1"/>
+    <col min="12" max="12" width="15.6160714285714" customWidth="1"/>
+    <col min="13" max="17" width="13.9821428571429" customWidth="1"/>
+    <col min="18" max="18" width="16.0625" customWidth="1"/>
+    <col min="21" max="21" width="77.6696428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:16">
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="5:16">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="5:16">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="5:16">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="5:16">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="5:16">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="7:19">
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="5:19">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="5:19">
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <v>0.783</v>
+      </c>
+      <c r="G10">
+        <v>0.474</v>
+      </c>
+      <c r="H10">
+        <v>0.462</v>
+      </c>
+      <c r="I10">
+        <v>0.24</v>
+      </c>
+      <c r="J10">
+        <v>0.45</v>
+      </c>
+      <c r="K10">
+        <v>0.71</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="2">
+        <v>11498538</v>
+      </c>
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="5:21">
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>0.783</v>
+      </c>
+      <c r="G11">
+        <v>0.455</v>
+      </c>
+      <c r="H11">
+        <v>0.461</v>
+      </c>
+      <c r="I11">
+        <v>0.244</v>
+      </c>
+      <c r="J11">
+        <v>0.45</v>
+      </c>
+      <c r="K11">
+        <v>0.71</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="3">
+        <v>11498538</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="E2:P7"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add LogisticRegressionPipeline & XGBoostPipeline
</commit_message>
<xml_diff>
--- a/report/model_performane.xlsx
+++ b/report/model_performane.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
   <si>
     <t>Hit Rate</t>
   </si>
@@ -41,7 +41,8 @@
     <t>something is wrong</t>
   </si>
   <si>
-    <t>1. deepFM &amp; wide&amp;deep got the same result -&gt; data is to small ???</t>
+    <t>1. deepFM &amp; wide&amp;deep got the same result -&gt; data is to small ???
+2. one-hot -&gt; industry ？？</t>
   </si>
   <si>
     <t>logloss</t>
@@ -96,6 +97,27 @@
   </si>
   <si>
     <t>deep part feature</t>
+  </si>
+  <si>
+    <t>Logistic regression with Ordinal Encode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1 regularization; </t>
+  </si>
+  <si>
+    <t>Logistic regression with One hot encode</t>
+  </si>
+  <si>
+    <t>out of memory for local computer</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>XGB + LR</t>
+  </si>
+  <si>
+    <t>DSSM</t>
   </si>
   <si>
     <t>deepFM</t>
@@ -121,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -149,10 +171,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -164,16 +202,84 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,90 +293,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -294,61 +316,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,121 +472,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,6 +515,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,22 +547,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,11 +578,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,145 +612,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -740,19 +762,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1082,11 +1104,11 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
   <sheetData>
     <row r="7" spans="8:10">
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="6:10">
       <c r="F8" t="s">
@@ -1145,15 +1167,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="E2:U11"/>
+  <dimension ref="E2:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
   <cols>
-    <col min="5" max="5" width="12.9375" customWidth="1"/>
+    <col min="5" max="5" width="34.6785714285714" customWidth="1"/>
     <col min="9" max="9" width="14.875" customWidth="1"/>
     <col min="12" max="12" width="15.6160714285714" customWidth="1"/>
     <col min="13" max="17" width="13.9821428571429" customWidth="1"/>
@@ -1165,104 +1187,104 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="5:16">
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="5:16">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="5:16">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="5:16">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" spans="5:16">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="7:19">
       <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1" t="s">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S8" s="1"/>
+      <c r="S8" s="2"/>
     </row>
     <row r="9" spans="5:19">
       <c r="E9" t="s">
@@ -1311,101 +1333,162 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="5:19">
+    <row r="10" spans="5:12">
       <c r="E10" t="s">
         <v>27</v>
       </c>
       <c r="F10">
+        <v>0.575</v>
+      </c>
+      <c r="I10">
+        <v>0.263</v>
+      </c>
+      <c r="J10">
+        <v>0.29</v>
+      </c>
+      <c r="K10">
+        <v>0.55</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="5:20">
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="T11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12">
+        <v>0.781</v>
+      </c>
+      <c r="G12">
+        <v>0.561</v>
+      </c>
+      <c r="H12">
+        <v>0.563</v>
+      </c>
+      <c r="I12">
+        <v>0.498</v>
+      </c>
+      <c r="J12">
+        <v>0.44</v>
+      </c>
+      <c r="K12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5">
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5">
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="5:19">
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15">
         <v>0.783</v>
       </c>
-      <c r="G10">
+      <c r="G15">
         <v>0.474</v>
       </c>
-      <c r="H10">
+      <c r="H15">
         <v>0.462</v>
       </c>
-      <c r="I10">
+      <c r="I15">
         <v>0.24</v>
       </c>
-      <c r="J10">
+      <c r="J15">
         <v>0.45</v>
       </c>
-      <c r="K10">
+      <c r="K15">
         <v>0.71</v>
       </c>
-      <c r="L10">
+      <c r="L15">
         <v>2</v>
       </c>
-      <c r="M10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10">
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15">
         <v>0</v>
       </c>
-      <c r="O10" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" s="2">
+      <c r="O15" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="3">
         <v>11498538</v>
       </c>
-      <c r="Q10">
+      <c r="Q15">
         <v>4</v>
       </c>
-      <c r="R10" t="s">
-        <v>30</v>
-      </c>
-      <c r="S10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="5:21">
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11">
+      <c r="R15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="5:21">
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16">
         <v>0.783</v>
       </c>
-      <c r="G11">
+      <c r="G16">
         <v>0.455</v>
       </c>
-      <c r="H11">
+      <c r="H16">
         <v>0.461</v>
       </c>
-      <c r="I11">
+      <c r="I16">
         <v>0.244</v>
       </c>
-      <c r="J11">
+      <c r="J16">
         <v>0.45</v>
       </c>
-      <c r="K11">
+      <c r="K16">
         <v>0.71</v>
       </c>
-      <c r="L11">
+      <c r="L16">
         <v>2</v>
       </c>
-      <c r="M11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11">
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16">
         <v>0</v>
       </c>
-      <c r="O11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" s="3">
+      <c r="O16" t="s">
+        <v>36</v>
+      </c>
+      <c r="P16" s="4">
         <v>11498538</v>
       </c>
-      <c r="Q11">
+      <c r="Q16">
         <v>4</v>
       </c>
-      <c r="R11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="U11" t="s">
-        <v>32</v>
+      <c r="R16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U16" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create custom XGB transformer
</commit_message>
<xml_diff>
--- a/report/model_performane.xlsx
+++ b/report/model_performane.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>Hit Rate</t>
   </si>
@@ -55,6 +55,9 @@
     <t>features</t>
   </si>
   <si>
+    <t>version</t>
+  </si>
+  <si>
     <t xml:space="preserve">model </t>
   </si>
   <si>
@@ -132,17 +135,23 @@
 3. L1 regularization</t>
   </si>
   <si>
+    <t>LR_1116_criteo_DenseBinStand_CateOnehotSVD</t>
+  </si>
+  <si>
     <t>1. sparse features -&gt; one-hot encode + TruncatedSVD(50) 
 2. dense feature -&gt; StandardScaler+KBinsDiscretizer
 3. L1 regularization</t>
   </si>
   <si>
+    <t>LR_1116_criteo_DenseBin_CateOnehotSVD</t>
+  </si>
+  <si>
     <t>1. sparse features -&gt; one-hot encode + TruncatedSVD(50) 
 2. dense feature -&gt; KBinsDiscretizer
 3. L1 regularization</t>
   </si>
   <si>
-    <t>???</t>
+    <t>LR_one_hot_1108_criteo</t>
   </si>
   <si>
     <t>1. sparse features -&gt; one-hot encode + TruncatedSVD(50) 
@@ -153,11 +162,42 @@
     <t>XGBoost</t>
   </si>
   <si>
+    <t>1. 1. all features are feeded into XBGoost: sparse -&gt; OrdinalEncoder</t>
+  </si>
+  <si>
+    <t>xgblr_1116_criteo</t>
+  </si>
+  <si>
     <t>XGB + LR</t>
   </si>
   <si>
-    <t>1. all features are feeded into XBGoost
-2. the leaves information are then feeded into LR</t>
+    <t>1. all features are feeded into XBGoost: sparse -&gt; OrdinalEncoder
+2. the leaves information are then feeded into LR -&gt; OneHotEncoder</t>
+  </si>
+  <si>
+    <t>xgblr2_1116_criteo</t>
+  </si>
+  <si>
+    <t>XGB+LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  dense features are feeded into XBGoost: OrdinalEncode
+2. the leaves information + dense +sparse features are then feeded into LR
+     1. leave info: OneHotEncoder
+     2. dense features: StandardScaler + KBinsDiscreizer
+     3. sparse features: OneHotEncoder + TruncatedSVD(50)
+</t>
+  </si>
+  <si>
+    <t>xgblr3_1116_criteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  All features are feeded into XBGoost: OrdinalEncode
+2. the leaves information + dense +sparse features are then feeded into LR
+     1. leave info: OneHotEncoder
+     2. dense features: StandardScaler + KBinsDiscreizer
+     3. sparse features: OneHotEncoder + TruncatedSVD(50)
+</t>
   </si>
   <si>
     <t>DSSM</t>
@@ -191,7 +231,7 @@
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,6 +242,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF92D050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -662,152 +709,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -825,6 +872,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1232,14 +1282,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="D2:V21"/>
+  <dimension ref="D2:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
   <cols>
+    <col min="4" max="4" width="17.5892857142857" customWidth="1"/>
     <col min="5" max="6" width="63.9821428571429" customWidth="1"/>
     <col min="10" max="10" width="14.875" customWidth="1"/>
     <col min="13" max="13" width="15.6160714285714" customWidth="1"/>
@@ -1357,62 +1408,65 @@
       </c>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="5:20">
+    <row r="9" spans="4:20">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" ht="53" spans="5:12">
       <c r="E10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G10">
         <v>0.575</v>
@@ -1429,10 +1483,10 @@
     </row>
     <row r="11" ht="53" spans="5:12">
       <c r="E11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11">
         <v>0.517</v>
@@ -1446,13 +1500,13 @@
     </row>
     <row r="12" ht="71" spans="5:21">
       <c r="E12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1461,15 +1515,15 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="U12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" ht="53" spans="5:12">
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G13">
         <v>0.721</v>
@@ -1481,14 +1535,17 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="53" spans="5:12">
+    <row r="14" customFormat="1" ht="53" spans="4:12">
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14">
+        <v>37</v>
+      </c>
+      <c r="G14" s="6">
         <v>0.732</v>
       </c>
       <c r="K14">
@@ -1498,12 +1555,15 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="15" customFormat="1" ht="53" spans="5:12">
+    <row r="15" customFormat="1" ht="53" spans="4:12">
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G15">
         <v>0.731</v>
@@ -1517,13 +1577,13 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="53" spans="4:12">
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="G16" s="1">
         <v>0.587</v>
@@ -1537,9 +1597,12 @@
     </row>
     <row r="17" spans="5:12">
       <c r="E17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="6">
         <v>0.771</v>
       </c>
       <c r="K17">
@@ -1549,12 +1612,15 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" ht="36" spans="5:12">
+    <row r="18" ht="36" spans="4:12">
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
       <c r="E18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="G18">
         <v>0.774</v>
@@ -1566,114 +1632,173 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" ht="124" spans="4:12">
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
       <c r="E19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="5:20">
+        <v>48</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19">
+        <v>0.743</v>
+      </c>
+      <c r="K19">
+        <v>0.41</v>
+      </c>
+      <c r="L19">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="20" ht="124" spans="4:12">
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="G20">
+        <v>0.774</v>
+      </c>
+      <c r="K20">
+        <v>0.44</v>
+      </c>
+      <c r="L20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="5:20">
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="6">
         <v>0.783</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>0.474</v>
       </c>
-      <c r="I20">
+      <c r="I22">
         <v>0.462</v>
       </c>
-      <c r="J20">
+      <c r="J22">
         <v>0.24</v>
       </c>
-      <c r="K20">
+      <c r="K22">
         <v>0.45</v>
       </c>
-      <c r="L20">
+      <c r="L22">
         <v>0.71</v>
       </c>
-      <c r="M20">
+      <c r="M22">
         <v>2</v>
       </c>
-      <c r="N20" t="s">
-        <v>44</v>
-      </c>
-      <c r="O20">
+      <c r="N22" t="s">
+        <v>54</v>
+      </c>
+      <c r="O22">
         <v>0</v>
       </c>
-      <c r="P20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q20" s="8">
+      <c r="P22" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q22" s="9">
         <v>11498538</v>
       </c>
-      <c r="R20">
+      <c r="R22">
         <v>4</v>
       </c>
-      <c r="S20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="5:22">
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21">
+      <c r="S22" t="s">
+        <v>56</v>
+      </c>
+      <c r="T22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="5:22">
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="6">
         <v>0.783</v>
       </c>
-      <c r="H21">
+      <c r="H23">
         <v>0.455</v>
       </c>
-      <c r="I21">
+      <c r="I23">
         <v>0.461</v>
       </c>
-      <c r="J21">
+      <c r="J23">
         <v>0.244</v>
       </c>
-      <c r="K21">
+      <c r="K23">
         <v>0.45</v>
       </c>
-      <c r="L21">
+      <c r="L23">
         <v>0.71</v>
       </c>
-      <c r="M21">
+      <c r="M23">
         <v>2</v>
       </c>
-      <c r="N21" t="s">
-        <v>44</v>
-      </c>
-      <c r="O21">
+      <c r="N23" t="s">
+        <v>54</v>
+      </c>
+      <c r="O23">
         <v>0</v>
       </c>
-      <c r="P21" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q21" s="9">
+      <c r="P23" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q23" s="10">
         <v>11498538</v>
       </c>
-      <c r="R21">
+      <c r="R23">
         <v>4</v>
       </c>
-      <c r="S21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="T21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="V21" t="s">
-        <v>48</v>
-      </c>
+      <c r="S23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="V23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6">
+      <c r="E35" s="5">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="5:6">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="5:6">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="5:6">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="M8:Q8"/>
     <mergeCell ref="S8:T8"/>
     <mergeCell ref="G12:M12"/>
     <mergeCell ref="E2:Q7"/>
+    <mergeCell ref="E35:F38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
deepFM dense feature decritizer
</commit_message>
<xml_diff>
--- a/report/model_performane.xlsx
+++ b/report/model_performane.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="11720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
   <si>
     <t>Hit Rate</t>
   </si>
@@ -215,6 +215,13 @@
     <t>26 sparse + 13 dense</t>
   </si>
   <si>
+    <t>deepFM_1125_criteo</t>
+  </si>
+  <si>
+    <t>1. sparse feature 
+2. dense feature -&gt;  KBinsDiscretizer(n_bins=20, encode='ordinal')</t>
+  </si>
+  <si>
     <t>wide &amp; deep</t>
   </si>
   <si>
@@ -226,12 +233,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +255,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="Monaco"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -263,6 +276,128 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,128 +410,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -419,181 +432,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,16 +633,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,21 +668,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -675,17 +679,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -704,129 +697,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -835,22 +848,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -861,6 +874,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -870,10 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1219,11 +1232,11 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
   <sheetData>
     <row r="7" spans="8:10">
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="6:10">
       <c r="F8" t="s">
@@ -1282,10 +1295,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="D2:V38"/>
+  <dimension ref="D2:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
@@ -1300,113 +1313,113 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:17">
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="5:17">
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="5:17">
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="5:17">
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="5:17">
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="5:17">
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="8:20">
       <c r="H8" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3" t="s">
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="T8" s="3"/>
+      <c r="T8" s="4"/>
     </row>
     <row r="9" spans="4:20">
       <c r="D9" t="s">
@@ -1465,7 +1478,7 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G10">
@@ -1485,7 +1498,7 @@
       <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G11">
@@ -1502,18 +1515,18 @@
       <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
       <c r="U12" t="s">
         <v>34</v>
       </c>
@@ -1522,7 +1535,7 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G13">
@@ -1542,7 +1555,7 @@
       <c r="E14" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="6">
@@ -1562,7 +1575,7 @@
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="5" t="s">
         <v>39</v>
       </c>
       <c r="G15">
@@ -1619,7 +1632,7 @@
       <c r="E18" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="5" t="s">
         <v>46</v>
       </c>
       <c r="G18">
@@ -1639,7 +1652,7 @@
       <c r="E19" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="5" t="s">
         <v>49</v>
       </c>
       <c r="G19">
@@ -1659,7 +1672,7 @@
       <c r="E20" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G20">
@@ -1724,21 +1737,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="5:22">
+    <row r="23" ht="36" spans="4:17">
+      <c r="D23" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="G23" s="6">
-        <v>0.783</v>
+        <v>0.788</v>
       </c>
       <c r="H23">
-        <v>0.455</v>
+        <v>0.469</v>
       </c>
       <c r="I23">
-        <v>0.461</v>
+        <v>0.459</v>
       </c>
       <c r="J23">
-        <v>0.244</v>
+        <v>0.27</v>
       </c>
       <c r="K23">
         <v>0.45</v>
@@ -1746,51 +1765,75 @@
       <c r="L23">
         <v>0.71</v>
       </c>
-      <c r="M23">
+      <c r="Q23" s="9"/>
+    </row>
+    <row r="24" spans="5:22">
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.783</v>
+      </c>
+      <c r="H24">
+        <v>0.455</v>
+      </c>
+      <c r="I24">
+        <v>0.461</v>
+      </c>
+      <c r="J24">
+        <v>0.244</v>
+      </c>
+      <c r="K24">
+        <v>0.45</v>
+      </c>
+      <c r="L24">
+        <v>0.71</v>
+      </c>
+      <c r="M24">
         <v>2</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N24" t="s">
         <v>54</v>
       </c>
-      <c r="O23">
+      <c r="O24">
         <v>0</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P24" t="s">
         <v>55</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q24" s="10">
         <v>11498538</v>
       </c>
-      <c r="R23">
+      <c r="R24">
         <v>4</v>
       </c>
-      <c r="S23" s="11" t="s">
+      <c r="S24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T23" s="11" t="s">
+      <c r="T24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="V23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6">
-      <c r="E35" s="5">
+      <c r="V24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
+      <c r="E36" s="4">
         <v>1</v>
       </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="5:6">
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="5:6">
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="5:6">
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="5:6">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1798,7 +1841,7 @@
     <mergeCell ref="S8:T8"/>
     <mergeCell ref="G12:M12"/>
     <mergeCell ref="E2:Q7"/>
-    <mergeCell ref="E35:F38"/>
+    <mergeCell ref="E36:F39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>